<commit_message>
[MastertList - QMM008] Upload
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM013.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM013.xlsx
@@ -44387,9 +44387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34:J35"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12"/>
   <cols>

</xml_diff>

<commit_message>
Update code QMM013 , QMM023
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM013.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM013.xlsx
@@ -122,7 +122,7 @@
     <definedName name="PG単価">[8]明細合計!#REF!</definedName>
     <definedName name="PG田中" localSheetId="0">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'マスタリスト '!$A$1:$L$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'マスタリスト '!$A$1:$L$40</definedName>
     <definedName name="PrintDaicho">[9]!PrintDaicho</definedName>
     <definedName name="QuitDaicho">[9]!QuitDaicho</definedName>
     <definedName name="SE単価" localSheetId="0">[8]明細合計!#REF!</definedName>
@@ -735,7 +735,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>11205</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>145677</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -44385,9 +44385,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K39"/>
+  <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12"/>
   <cols>
@@ -44857,28 +44859,40 @@
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="2:11" ht="13.15" customHeight="1">
-      <c r="B38" s="7"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
     </row>
     <row r="39" spans="2:11" ht="13.15" customHeight="1">
-      <c r="B39" s="8"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="2:11" ht="13.15" customHeight="1">
+      <c r="B40" s="8"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -44890,7 +44904,7 @@
     <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>